<commit_message>
Dashboard: adiciona 'TOP 5 Seller do mês' no app Lokok2 (view + Chart.js) e calcula monthlyResponsibles/topMonthOptions/selectedTopMonth/topManagerEntries na rota /dashboard
</commit_message>
<xml_diff>
--- a/data/Wholesale Suppliers and Product Opportunities.xlsx
+++ b/data/Wholesale Suppliers and Product Opportunities.xlsx
@@ -4,6 +4,9 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Wholesale LOKOK" sheetId="1" r:id="rId1"/>
+    <sheet name="Wholesale CANADA" sheetId="2" r:id="rId2"/>
+    <sheet name="Wholesale MEXICO" sheetId="3" r:id="rId3"/>
+    <sheet name="Wholesale CHINA" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -48677,4 +48680,358 @@
     <ignoredError numberStoredAsText="1" sqref="A1:AH1055"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Website</v>
+      </c>
+      <c r="C1" t="str">
+        <v>CATEGORÍA</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Account Request Status</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Responsable</v>
+      </c>
+      <c r="F1" t="str">
+        <v>STATUS (PENDING APPROVAL, BUYING, CHECKING, NOT COMPETITIVE, NOT INTERESTING, RED FLAG)</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Description/Notes</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Contact Name</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Contact Phone</v>
+      </c>
+      <c r="J1" t="str">
+        <v>E-Mail</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Address</v>
+      </c>
+      <c r="L1" t="str">
+        <v>User</v>
+      </c>
+      <c r="M1" t="str">
+        <v>PASSWORD</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Created_By_User_ID</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Created_By_User_Name</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Created_At</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>FORNECEDOR</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Updated_At</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Updated_By_User_Name</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Updated_By_User_ID</v>
+      </c>
+      <c r="U1" t="str">
+        <v>DATE</v>
+      </c>
+      <c r="V1" t="str">
+        <v>PRIO (1 - TOP, 5 - bajo)</v>
+      </c>
+      <c r="W1" t="str">
+        <v>LLAMAR</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Comments</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Priority: Monthly Revenue / SKU quantity</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Priority: Average FBA Sellers</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Priority: Average Sellers</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Priority: Amazon In Stock Rate</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Priority: Additional Information</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Priority: Who will call</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Priority: Call Date</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Priority: Result</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Priority: Follow-up Task</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Priority: Need Approval</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:AH1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Website</v>
+      </c>
+      <c r="C1" t="str">
+        <v>CATEGORÍA</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Account Request Status</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Responsable</v>
+      </c>
+      <c r="F1" t="str">
+        <v>STATUS (PENDING APPROVAL, BUYING, CHECKING, NOT COMPETITIVE, NOT INTERESTING, RED FLAG)</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Description/Notes</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Contact Name</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Contact Phone</v>
+      </c>
+      <c r="J1" t="str">
+        <v>E-Mail</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Address</v>
+      </c>
+      <c r="L1" t="str">
+        <v>User</v>
+      </c>
+      <c r="M1" t="str">
+        <v>PASSWORD</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Created_By_User_ID</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Created_By_User_Name</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Created_At</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>FORNECEDOR</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Updated_At</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Updated_By_User_Name</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Updated_By_User_ID</v>
+      </c>
+      <c r="U1" t="str">
+        <v>DATE</v>
+      </c>
+      <c r="V1" t="str">
+        <v>PRIO (1 - TOP, 5 - bajo)</v>
+      </c>
+      <c r="W1" t="str">
+        <v>LLAMAR</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Comments</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Priority: Monthly Revenue / SKU quantity</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Priority: Average FBA Sellers</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Priority: Average Sellers</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Priority: Amazon In Stock Rate</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Priority: Additional Information</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Priority: Who will call</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Priority: Call Date</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Priority: Result</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Priority: Follow-up Task</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Priority: Need Approval</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:AH1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Website</v>
+      </c>
+      <c r="C1" t="str">
+        <v>CATEGORÍA</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Account Request Status</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Responsable</v>
+      </c>
+      <c r="F1" t="str">
+        <v>STATUS (PENDING APPROVAL, BUYING, CHECKING, NOT COMPETITIVE, NOT INTERESTING, RED FLAG)</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Description/Notes</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Contact Name</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Contact Phone</v>
+      </c>
+      <c r="J1" t="str">
+        <v>E-Mail</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Address</v>
+      </c>
+      <c r="L1" t="str">
+        <v>User</v>
+      </c>
+      <c r="M1" t="str">
+        <v>PASSWORD</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Created_By_User_ID</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Created_By_User_Name</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Created_At</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>FORNECEDOR</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Updated_At</v>
+      </c>
+      <c r="S1" t="str">
+        <v>Updated_By_User_Name</v>
+      </c>
+      <c r="T1" t="str">
+        <v>Updated_By_User_ID</v>
+      </c>
+      <c r="U1" t="str">
+        <v>DATE</v>
+      </c>
+      <c r="V1" t="str">
+        <v>PRIO (1 - TOP, 5 - bajo)</v>
+      </c>
+      <c r="W1" t="str">
+        <v>LLAMAR</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Comments</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Priority: Monthly Revenue / SKU quantity</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Priority: Average FBA Sellers</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Priority: Average Sellers</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>Priority: Amazon In Stock Rate</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Priority: Additional Information</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Priority: Who will call</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Priority: Call Date</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Priority: Result</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Priority: Follow-up Task</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Priority: Need Approval</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:AH1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>